<commit_message>
fix: fk_id of tambon data
</commit_message>
<xml_diff>
--- a/xlsx/thai_geographies.xlsx
+++ b/xlsx/thai_geographies.xlsx
@@ -13,7 +13,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>ภาคเหนือ</t>
+  </si>
+  <si>
+    <t>ภาคกลาง</t>
+  </si>
+  <si>
+    <t>ภาคตะวันออกเฉียงเหนือ</t>
+  </si>
+  <si>
+    <t>ภาคตะวันตก</t>
+  </si>
+  <si>
+    <t>ภาคตะวันออก</t>
+  </si>
+  <si>
+    <t>ภาคใต้</t>
+  </si>
   <si>
     <t>id</t>
   </si>
@@ -80,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B14"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -139,6 +163,62 @@
         <v>7</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
format: re-format of generate data
</commit_message>
<xml_diff>
--- a/xlsx/thai_geographies.xlsx
+++ b/xlsx/thai_geographies.xlsx
@@ -13,31 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>ภาคเหนือ</t>
-  </si>
-  <si>
-    <t>ภาคกลาง</t>
-  </si>
-  <si>
-    <t>ภาคตะวันออกเฉียงเหนือ</t>
-  </si>
-  <si>
-    <t>ภาคตะวันตก</t>
-  </si>
-  <si>
-    <t>ภาคตะวันออก</t>
-  </si>
-  <si>
-    <t>ภาคใต้</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>id</t>
   </si>
@@ -104,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B7"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -163,62 +139,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>